<commit_message>
Changes to Repo due to Revision
</commit_message>
<xml_diff>
--- a/notebooks/df_relperc_leukgroup.xlsx
+++ b/notebooks/df_relperc_leukgroup.xlsx
@@ -37,10 +37,7 @@
     <t>B-Lymphocyte</t>
   </si>
   <si>
-    <t>HPSC</t>
-  </si>
-  <si>
-    <t>Initial</t>
+    <t>HSPCs</t>
   </si>
   <si>
     <t>K562</t>
@@ -49,16 +46,19 @@
     <t>KASUMI</t>
   </si>
   <si>
-    <t>KCL</t>
-  </si>
-  <si>
-    <t>PDX</t>
-  </si>
-  <si>
-    <t>PDX2</t>
-  </si>
-  <si>
-    <t>Relapse</t>
+    <t>KCL22</t>
+  </si>
+  <si>
+    <t>PDX1</t>
+  </si>
+  <si>
+    <t>PDX2ini</t>
+  </si>
+  <si>
+    <t>PDX2rel</t>
+  </si>
+  <si>
+    <t>PDX3</t>
   </si>
   <si>
     <t>SUPB15</t>
@@ -642,13 +642,13 @@
         <v>16</v>
       </c>
       <c r="D11">
-        <v>357</v>
+        <v>901</v>
       </c>
       <c r="E11">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="F11">
-        <v>7.282913165266107</v>
+        <v>8.435072142064373</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -662,13 +662,13 @@
         <v>17</v>
       </c>
       <c r="D12">
-        <v>1226</v>
+        <v>539</v>
       </c>
       <c r="E12">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F12">
-        <v>3.752039151712887</v>
+        <v>4.267161410018553</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -682,13 +682,13 @@
         <v>18</v>
       </c>
       <c r="D13">
-        <v>1066</v>
+        <v>449</v>
       </c>
       <c r="E13">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>4.878048780487805</v>
+        <v>4.89977728285078</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -702,13 +702,13 @@
         <v>16</v>
       </c>
       <c r="D14">
-        <v>901</v>
+        <v>2355</v>
       </c>
       <c r="E14">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="F14">
-        <v>8.435072142064373</v>
+        <v>1.443736730360934</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -722,13 +722,13 @@
         <v>17</v>
       </c>
       <c r="D15">
-        <v>539</v>
+        <v>1730</v>
       </c>
       <c r="E15">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F15">
-        <v>4.267161410018553</v>
+        <v>1.618497109826589</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -742,13 +742,13 @@
         <v>18</v>
       </c>
       <c r="D16">
-        <v>449</v>
+        <v>1033</v>
       </c>
       <c r="E16">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="F16">
-        <v>4.89977728285078</v>
+        <v>7.55082284607938</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -762,13 +762,13 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>2355</v>
+        <v>116</v>
       </c>
       <c r="E17">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F17">
-        <v>1.443736730360934</v>
+        <v>12.06896551724138</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -782,13 +782,13 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>1730</v>
+        <v>162</v>
       </c>
       <c r="E18">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="F18">
-        <v>1.618497109826589</v>
+        <v>3.08641975308642</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -802,13 +802,13 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>1033</v>
+        <v>628</v>
       </c>
       <c r="E19">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="F19">
-        <v>7.55082284607938</v>
+        <v>5.573248407643312</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -822,13 +822,13 @@
         <v>16</v>
       </c>
       <c r="D20">
-        <v>116</v>
+        <v>1791</v>
       </c>
       <c r="E20">
-        <v>14</v>
+        <v>306</v>
       </c>
       <c r="F20">
-        <v>12.06896551724138</v>
+        <v>17.08542713567839</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -842,13 +842,13 @@
         <v>17</v>
       </c>
       <c r="D21">
-        <v>162</v>
+        <v>977</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>234</v>
       </c>
       <c r="F21">
-        <v>3.08641975308642</v>
+        <v>23.95087001023541</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -862,13 +862,13 @@
         <v>18</v>
       </c>
       <c r="D22">
-        <v>628</v>
+        <v>686</v>
       </c>
       <c r="E22">
-        <v>35</v>
+        <v>169</v>
       </c>
       <c r="F22">
-        <v>5.573248407643312</v>
+        <v>24.63556851311953</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -882,13 +882,13 @@
         <v>16</v>
       </c>
       <c r="D23">
-        <v>1791</v>
+        <v>357</v>
       </c>
       <c r="E23">
-        <v>306</v>
+        <v>26</v>
       </c>
       <c r="F23">
-        <v>17.08542713567839</v>
+        <v>7.282913165266107</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -902,13 +902,13 @@
         <v>17</v>
       </c>
       <c r="D24">
-        <v>977</v>
+        <v>1226</v>
       </c>
       <c r="E24">
-        <v>234</v>
+        <v>46</v>
       </c>
       <c r="F24">
-        <v>23.95087001023541</v>
+        <v>3.752039151712887</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -922,13 +922,13 @@
         <v>18</v>
       </c>
       <c r="D25">
-        <v>686</v>
+        <v>1066</v>
       </c>
       <c r="E25">
-        <v>169</v>
+        <v>52</v>
       </c>
       <c r="F25">
-        <v>24.63556851311953</v>
+        <v>4.878048780487805</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -942,13 +942,13 @@
         <v>16</v>
       </c>
       <c r="D26">
-        <v>1198</v>
+        <v>221</v>
       </c>
       <c r="E26">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="F26">
-        <v>2.337228714524207</v>
+        <v>1.809954751131222</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -962,13 +962,13 @@
         <v>17</v>
       </c>
       <c r="D27">
-        <v>1492</v>
+        <v>650</v>
       </c>
       <c r="E27">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="F27">
-        <v>4.356568364611261</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -982,13 +982,13 @@
         <v>18</v>
       </c>
       <c r="D28">
-        <v>953</v>
+        <v>259</v>
       </c>
       <c r="E28">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="F28">
-        <v>7.345225603357817</v>
+        <v>7.335907335907336</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1002,13 +1002,13 @@
         <v>16</v>
       </c>
       <c r="D29">
-        <v>221</v>
+        <v>1198</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F29">
-        <v>1.809954751131222</v>
+        <v>2.337228714524207</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1022,13 +1022,13 @@
         <v>17</v>
       </c>
       <c r="D30">
-        <v>650</v>
+        <v>1492</v>
       </c>
       <c r="E30">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>4.356568364611261</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1042,13 +1042,13 @@
         <v>18</v>
       </c>
       <c r="D31">
-        <v>259</v>
+        <v>953</v>
       </c>
       <c r="E31">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="F31">
-        <v>7.335907335907336</v>
+        <v>7.345225603357817</v>
       </c>
     </row>
     <row r="32" spans="1:6">

</xml_diff>